<commit_message>
Initial working version for labelling workouts
</commit_message>
<xml_diff>
--- a/data/walk_groups.xlsx
+++ b/data/walk_groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>walk_group</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Bay Run</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -98,13 +101,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -452,7 +455,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -470,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -478,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -486,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -494,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -502,7 +505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -510,7 +513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -518,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -526,7 +529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -534,7 +537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -548,6 +551,14 @@
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>